<commit_message>
Atualizando status das tarefas no Backlog
</commit_message>
<xml_diff>
--- a/documentacao/excel/backlog-Grupo-01.xlsx
+++ b/documentacao/excel/backlog-Grupo-01.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bb9df5b836737798/Área de Trabalho/sptech - 1° semestre/{2ª SPRINT}/projeto-pi-sprint-1/documentacao/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Documents\github\projeto-pi-sprint-2\documentacao\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{B12A43B0-AE25-4F8E-AAB5-EA991842DA8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EA1183F-8913-491D-A2E1-86E332C8560F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B327DC7-B96A-456E-9FA2-324D59BE18BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7393E741-8B86-48EF-BE07-B24862E557C3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7393E741-8B86-48EF-BE07-B24862E557C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="100">
   <si>
     <t>Backlog</t>
   </si>
@@ -336,6 +336,9 @@
   </si>
   <si>
     <t>Planejado</t>
+  </si>
+  <si>
+    <t>Ok</t>
   </si>
 </sst>
 </file>
@@ -555,7 +558,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -671,6 +674,9 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -680,8 +686,11 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2046,8 +2055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E230A6-6E41-41E9-834E-469679204ECD}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2071,18 +2080,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="41"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
@@ -2123,10 +2132,10 @@
       </c>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
-      <c r="M2" s="42" t="s">
+      <c r="M2" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="N2" s="42" t="s">
+      <c r="N2" s="39" t="s">
         <v>98</v>
       </c>
       <c r="P2" s="4"/>
@@ -2274,13 +2283,13 @@
       <c r="D6" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="F6" s="37">
+      <c r="F6" s="43">
         <v>13</v>
       </c>
-      <c r="G6" s="37">
+      <c r="G6" s="43">
         <v>1</v>
       </c>
       <c r="H6" s="15">
@@ -2317,13 +2326,13 @@
       <c r="D7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="37" t="s">
+      <c r="E7" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="F7" s="37">
+      <c r="F7" s="43">
         <v>8</v>
       </c>
-      <c r="G7" s="37">
+      <c r="G7" s="43">
         <v>2</v>
       </c>
       <c r="H7" s="12">
@@ -2359,13 +2368,13 @@
       <c r="D8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="37" t="s">
+      <c r="E8" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="F8" s="37">
+      <c r="F8" s="43">
         <v>13</v>
       </c>
-      <c r="G8" s="37">
+      <c r="G8" s="43">
         <v>2</v>
       </c>
       <c r="H8" s="12">
@@ -2400,13 +2409,13 @@
       <c r="D9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="37" t="s">
+      <c r="E9" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="F9" s="37">
+      <c r="F9" s="43">
         <v>5</v>
       </c>
-      <c r="G9" s="37">
+      <c r="G9" s="43">
         <v>1</v>
       </c>
       <c r="H9" s="12">
@@ -2434,13 +2443,13 @@
       <c r="D10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="E10" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="37">
+      <c r="F10" s="43">
         <v>5</v>
       </c>
-      <c r="G10" s="37">
+      <c r="G10" s="43">
         <v>2</v>
       </c>
       <c r="H10" s="12">
@@ -2472,13 +2481,13 @@
       <c r="D11" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="37" t="s">
+      <c r="E11" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="F11" s="37">
+      <c r="F11" s="43">
         <v>5</v>
       </c>
-      <c r="G11" s="37">
+      <c r="G11" s="43">
         <v>3</v>
       </c>
       <c r="H11" s="12">
@@ -2506,13 +2515,13 @@
       <c r="D12" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="37" t="s">
+      <c r="E12" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="F12" s="37">
+      <c r="F12" s="43">
         <v>3</v>
       </c>
-      <c r="G12" s="37">
+      <c r="G12" s="43">
         <v>3</v>
       </c>
       <c r="H12" s="18">
@@ -2540,13 +2549,13 @@
       <c r="D13" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="37" t="s">
+      <c r="E13" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="37">
+      <c r="F13" s="43">
         <v>5</v>
       </c>
-      <c r="G13" s="37">
+      <c r="G13" s="43">
         <v>1</v>
       </c>
       <c r="H13" s="31">
@@ -2562,205 +2571,205 @@
       <c r="N13" s="5"/>
     </row>
     <row r="14" spans="1:16" ht="34.799999999999997" x14ac:dyDescent="0.3">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14" s="30">
         <v>2</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="D14" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="37" t="s">
+      <c r="E14" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="F14" s="37">
+      <c r="F14" s="43">
         <v>13</v>
       </c>
-      <c r="G14" s="37">
+      <c r="G14" s="43">
         <v>1</v>
       </c>
-      <c r="H14" s="25">
+      <c r="H14" s="31">
         <v>45596</v>
       </c>
-      <c r="I14" s="24" t="s">
+      <c r="I14" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="J14" s="24" t="s">
-        <v>10</v>
+      <c r="J14" s="30" t="s">
+        <v>81</v>
       </c>
       <c r="K14" s="6"/>
       <c r="N14" s="5"/>
     </row>
     <row r="15" spans="1:16" ht="34.799999999999997" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="24">
+      <c r="C15" s="30">
         <v>2</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="37" t="s">
+      <c r="E15" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="F15" s="37">
+      <c r="F15" s="43">
         <v>8</v>
       </c>
-      <c r="G15" s="37">
+      <c r="G15" s="43">
         <v>2</v>
       </c>
-      <c r="H15" s="25">
+      <c r="H15" s="31">
         <v>45596</v>
       </c>
-      <c r="I15" s="24" t="s">
+      <c r="I15" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="J15" s="24" t="s">
-        <v>10</v>
+      <c r="J15" s="30" t="s">
+        <v>99</v>
       </c>
       <c r="K15" s="6"/>
       <c r="N15" s="5"/>
     </row>
     <row r="16" spans="1:16" ht="34.799999999999997" x14ac:dyDescent="0.3">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="24">
+      <c r="C16" s="30">
         <v>2</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="D16" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="37" t="s">
+      <c r="E16" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="F16" s="37">
+      <c r="F16" s="43">
         <v>13</v>
       </c>
-      <c r="G16" s="37">
+      <c r="G16" s="43">
         <v>2</v>
       </c>
-      <c r="H16" s="25">
+      <c r="H16" s="31">
         <v>45596</v>
       </c>
-      <c r="I16" s="24" t="s">
+      <c r="I16" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="J16" s="24" t="s">
-        <v>10</v>
+      <c r="J16" s="30" t="s">
+        <v>81</v>
       </c>
       <c r="K16" s="1"/>
       <c r="N16" s="5"/>
     </row>
     <row r="17" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="24">
+      <c r="C17" s="30">
         <v>2</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="D17" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="37" t="s">
+      <c r="E17" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="F17" s="37">
+      <c r="F17" s="43">
         <v>8</v>
       </c>
-      <c r="G17" s="37">
+      <c r="G17" s="43">
         <v>2</v>
       </c>
-      <c r="H17" s="25">
+      <c r="H17" s="31">
         <v>45596</v>
       </c>
-      <c r="I17" s="24" t="s">
+      <c r="I17" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="J17" s="24" t="s">
-        <v>10</v>
+      <c r="J17" s="30" t="s">
+        <v>81</v>
       </c>
       <c r="K17" s="1"/>
       <c r="N17" s="5"/>
     </row>
     <row r="18" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="C18" s="24">
+      <c r="C18" s="30">
         <v>2</v>
       </c>
-      <c r="D18" s="24" t="s">
+      <c r="D18" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="37" t="s">
+      <c r="E18" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="F18" s="37">
+      <c r="F18" s="43">
         <v>8</v>
       </c>
-      <c r="G18" s="37">
+      <c r="G18" s="43">
         <v>2</v>
       </c>
-      <c r="H18" s="25">
+      <c r="H18" s="31">
         <v>45597</v>
       </c>
-      <c r="I18" s="24" t="s">
+      <c r="I18" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="24" t="s">
-        <v>10</v>
+      <c r="J18" s="30" t="s">
+        <v>81</v>
       </c>
       <c r="K18" s="1"/>
       <c r="N18" s="5"/>
     </row>
     <row r="19" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.3">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="24">
+      <c r="C19" s="30">
         <v>2</v>
       </c>
-      <c r="D19" s="24" t="s">
+      <c r="D19" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="37" t="s">
+      <c r="E19" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="F19" s="37">
+      <c r="F19" s="43">
         <v>8</v>
       </c>
-      <c r="G19" s="37">
+      <c r="G19" s="43">
         <v>2</v>
       </c>
-      <c r="H19" s="25">
+      <c r="H19" s="31">
         <v>45596</v>
       </c>
-      <c r="I19" s="24" t="s">
+      <c r="I19" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="24" t="s">
-        <v>10</v>
+      <c r="J19" s="30" t="s">
+        <v>81</v>
       </c>
       <c r="K19" s="1"/>
       <c r="N19" s="5"/>
@@ -2778,13 +2787,13 @@
       <c r="D20" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="37" t="s">
+      <c r="E20" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="F20" s="37">
+      <c r="F20" s="43">
         <v>5</v>
       </c>
-      <c r="G20" s="37">
+      <c r="G20" s="43">
         <v>1</v>
       </c>
       <c r="H20" s="12">
@@ -2798,195 +2807,195 @@
       </c>
     </row>
     <row r="21" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.3">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="24">
+      <c r="C21" s="30">
         <v>2</v>
       </c>
-      <c r="D21" s="24" t="s">
+      <c r="D21" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="37" t="s">
+      <c r="E21" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="F21" s="37">
+      <c r="F21" s="43">
         <v>8</v>
       </c>
-      <c r="G21" s="37">
+      <c r="G21" s="43">
         <v>1</v>
       </c>
-      <c r="H21" s="25">
+      <c r="H21" s="31">
         <v>45631</v>
       </c>
-      <c r="I21" s="24" t="s">
+      <c r="I21" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="J21" s="24" t="s">
-        <v>10</v>
+      <c r="J21" s="30" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.3">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="24">
+      <c r="C22" s="30">
         <v>2</v>
       </c>
-      <c r="D22" s="24" t="s">
+      <c r="D22" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="37" t="s">
+      <c r="E22" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="F22" s="37">
+      <c r="F22" s="43">
         <v>8</v>
       </c>
-      <c r="G22" s="37">
+      <c r="G22" s="43">
         <v>2</v>
       </c>
-      <c r="H22" s="25">
+      <c r="H22" s="31">
         <v>45596</v>
       </c>
-      <c r="I22" s="24" t="s">
+      <c r="I22" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="J22" s="24" t="s">
-        <v>10</v>
+      <c r="J22" s="30" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.3">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="24">
+      <c r="C23" s="30">
         <v>2</v>
       </c>
-      <c r="D23" s="24" t="s">
+      <c r="D23" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="37" t="s">
+      <c r="E23" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="F23" s="37">
+      <c r="F23" s="43">
         <v>8</v>
       </c>
-      <c r="G23" s="37">
+      <c r="G23" s="43">
         <v>3</v>
       </c>
-      <c r="H23" s="25">
+      <c r="H23" s="31">
         <v>45596</v>
       </c>
-      <c r="I23" s="24" t="s">
+      <c r="I23" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="J23" s="24" t="s">
-        <v>10</v>
+      <c r="J23" s="30" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.3">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="24">
+      <c r="C24" s="30">
         <v>2</v>
       </c>
-      <c r="D24" s="24" t="s">
+      <c r="D24" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="37" t="s">
+      <c r="E24" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="F24" s="37">
+      <c r="F24" s="43">
         <v>13</v>
       </c>
-      <c r="G24" s="37">
+      <c r="G24" s="43">
         <v>3</v>
       </c>
-      <c r="H24" s="25">
+      <c r="H24" s="31">
         <v>45596</v>
       </c>
-      <c r="I24" s="24" t="s">
+      <c r="I24" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="J24" s="24" t="s">
-        <v>10</v>
+      <c r="J24" s="30" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.3">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="24">
+      <c r="C25" s="30">
         <v>2</v>
       </c>
-      <c r="D25" s="24" t="s">
+      <c r="D25" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="37" t="s">
+      <c r="E25" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="F25" s="37">
+      <c r="F25" s="43">
         <v>13</v>
       </c>
-      <c r="G25" s="37">
+      <c r="G25" s="43">
         <v>3</v>
       </c>
-      <c r="H25" s="25">
+      <c r="H25" s="31">
         <v>45596</v>
       </c>
-      <c r="I25" s="24" t="s">
+      <c r="I25" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="J25" s="24" t="s">
-        <v>10</v>
+      <c r="J25" s="30" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.3">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="24">
+      <c r="C26" s="30">
         <v>2</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="D26" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="37" t="s">
+      <c r="E26" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="F26" s="37">
+      <c r="F26" s="43">
         <v>8</v>
       </c>
-      <c r="G26" s="37">
+      <c r="G26" s="43">
         <v>3</v>
       </c>
-      <c r="H26" s="25">
+      <c r="H26" s="31">
         <v>45596</v>
       </c>
-      <c r="I26" s="24" t="s">
+      <c r="I26" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="J26" s="24" t="s">
-        <v>82</v>
+      <c r="J26" s="30" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -3254,15 +3263,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD11765F9AC0004AAF0A4CAAFDFAF16A" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b51fd1e8b3b325edc2e3e5af1016e876">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9fdc8751-6fef-42ec-b05c-835dd8c535b4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f375ab854fe714e6d25c0e520c080200" ns3:_="">
     <xsd:import namespace="9fdc8751-6fef-42ec-b05c-835dd8c535b4"/>
@@ -3438,6 +3438,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3445,14 +3454,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{085FFE83-7874-4863-A9C7-9C338481B563}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA33053E-EA8F-437C-9F67-47A4F0BC10D0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3466,6 +3467,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{085FFE83-7874-4863-A9C7-9C338481B563}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
subindo ppt quase completo
</commit_message>
<xml_diff>
--- a/documentacao/excel/backlog-Grupo-01.xlsx
+++ b/documentacao/excel/backlog-Grupo-01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Documents\github\projeto-pi-sprint-2\documentacao\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bb9df5b836737798/Área de Trabalho/sptech - 1° semestre/3a sprint/projeto-pi-sprint-3/documentacao/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B327DC7-B96A-456E-9FA2-324D59BE18BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{9B327DC7-B96A-456E-9FA2-324D59BE18BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A5CB9B6-FC9F-4B9E-B9B7-FA00D3D677AE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7393E741-8B86-48EF-BE07-B24862E557C3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7393E741-8B86-48EF-BE07-B24862E557C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -677,6 +677,12 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -685,12 +691,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -814,48 +814,11 @@
           <c:cat>
             <c:strRef>
               <c:f>Planilha1!$L$3:$L$7</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>TOTAL</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>SP1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>SP2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>SP3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>SP4</c:v>
-                </c:pt>
-              </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Planilha1!$N$3:$N$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>309</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>93</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>104</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>112</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -886,48 +849,11 @@
           <c:cat>
             <c:strRef>
               <c:f>Planilha1!$L$3:$L$7</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>TOTAL</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>SP1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>SP2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>SP3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>SP4</c:v>
-                </c:pt>
-              </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Planilha1!$M$3:$M$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>322</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>126</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>115</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -945,6 +871,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="555575504"/>
         <c:axId val="555568304"/>
@@ -2053,10 +1980,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E230A6-6E41-41E9-834E-469679204ECD}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2080,18 +2008,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="44"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
@@ -2140,7 +2068,7 @@
       </c>
       <c r="P2" s="4"/>
     </row>
-    <row r="3" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="32.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
         <v>7</v>
       </c>
@@ -2184,7 +2112,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="34.799999999999997" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="34.799999999999997" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="32" t="s">
         <v>69</v>
       </c>
@@ -2227,7 +2155,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="34.799999999999997" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="34.799999999999997" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="32" t="s">
         <v>12</v>
       </c>
@@ -2270,7 +2198,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="34.799999999999997" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="34.799999999999997" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="33" t="s">
         <v>13</v>
       </c>
@@ -2283,13 +2211,13 @@
       <c r="D6" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="43" t="s">
+      <c r="E6" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="F6" s="43">
+      <c r="F6" s="40">
         <v>13</v>
       </c>
-      <c r="G6" s="43">
+      <c r="G6" s="40">
         <v>1</v>
       </c>
       <c r="H6" s="15">
@@ -2313,7 +2241,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="34.799999999999997" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="34.799999999999997" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="34" t="s">
         <v>15</v>
       </c>
@@ -2326,13 +2254,13 @@
       <c r="D7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="F7" s="43">
+      <c r="F7" s="40">
         <v>8</v>
       </c>
-      <c r="G7" s="43">
+      <c r="G7" s="40">
         <v>2</v>
       </c>
       <c r="H7" s="12">
@@ -2355,7 +2283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="34.799999999999997" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="34.799999999999997" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="34" t="s">
         <v>76</v>
       </c>
@@ -2368,13 +2296,13 @@
       <c r="D8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="43" t="s">
+      <c r="E8" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="F8" s="43">
+      <c r="F8" s="40">
         <v>13</v>
       </c>
-      <c r="G8" s="43">
+      <c r="G8" s="40">
         <v>2</v>
       </c>
       <c r="H8" s="12">
@@ -2396,7 +2324,7 @@
       </c>
       <c r="N8" s="5"/>
     </row>
-    <row r="9" spans="1:16" ht="34.799999999999997" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="34.799999999999997" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="34" t="s">
         <v>18</v>
       </c>
@@ -2409,13 +2337,13 @@
       <c r="D9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="43" t="s">
+      <c r="E9" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="F9" s="43">
+      <c r="F9" s="40">
         <v>5</v>
       </c>
-      <c r="G9" s="43">
+      <c r="G9" s="40">
         <v>1</v>
       </c>
       <c r="H9" s="12">
@@ -2430,7 +2358,7 @@
       <c r="K9" s="1"/>
       <c r="N9" s="5"/>
     </row>
-    <row r="10" spans="1:16" ht="34.799999999999997" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="34.799999999999997" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="34" t="s">
         <v>19</v>
       </c>
@@ -2443,13 +2371,13 @@
       <c r="D10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="43" t="s">
+      <c r="E10" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="43">
+      <c r="F10" s="40">
         <v>5</v>
       </c>
-      <c r="G10" s="43">
+      <c r="G10" s="40">
         <v>2</v>
       </c>
       <c r="H10" s="12">
@@ -2468,7 +2396,7 @@
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
     </row>
-    <row r="11" spans="1:16" ht="34.799999999999997" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="34.799999999999997" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="34" t="s">
         <v>79</v>
       </c>
@@ -2481,13 +2409,13 @@
       <c r="D11" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="43" t="s">
+      <c r="E11" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="F11" s="43">
+      <c r="F11" s="40">
         <v>5</v>
       </c>
-      <c r="G11" s="43">
+      <c r="G11" s="40">
         <v>3</v>
       </c>
       <c r="H11" s="12">
@@ -2502,7 +2430,7 @@
       <c r="K11" s="1"/>
       <c r="N11" s="5"/>
     </row>
-    <row r="12" spans="1:16" ht="34.799999999999997" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="34.799999999999997" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="35" t="s">
         <v>20</v>
       </c>
@@ -2515,13 +2443,13 @@
       <c r="D12" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="43" t="s">
+      <c r="E12" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="F12" s="43">
+      <c r="F12" s="40">
         <v>3</v>
       </c>
-      <c r="G12" s="43">
+      <c r="G12" s="40">
         <v>3</v>
       </c>
       <c r="H12" s="18">
@@ -2549,13 +2477,13 @@
       <c r="D13" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="43" t="s">
+      <c r="E13" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="43">
+      <c r="F13" s="40">
         <v>5</v>
       </c>
-      <c r="G13" s="43">
+      <c r="G13" s="40">
         <v>1</v>
       </c>
       <c r="H13" s="31">
@@ -2583,13 +2511,13 @@
       <c r="D14" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="43" t="s">
+      <c r="E14" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="F14" s="43">
+      <c r="F14" s="40">
         <v>13</v>
       </c>
-      <c r="G14" s="43">
+      <c r="G14" s="40">
         <v>1</v>
       </c>
       <c r="H14" s="31">
@@ -2617,13 +2545,13 @@
       <c r="D15" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="43" t="s">
+      <c r="E15" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="F15" s="43">
+      <c r="F15" s="40">
         <v>8</v>
       </c>
-      <c r="G15" s="43">
+      <c r="G15" s="40">
         <v>2</v>
       </c>
       <c r="H15" s="31">
@@ -2651,13 +2579,13 @@
       <c r="D16" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="43" t="s">
+      <c r="E16" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="F16" s="43">
+      <c r="F16" s="40">
         <v>13</v>
       </c>
-      <c r="G16" s="43">
+      <c r="G16" s="40">
         <v>2</v>
       </c>
       <c r="H16" s="31">
@@ -2685,13 +2613,13 @@
       <c r="D17" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="43" t="s">
+      <c r="E17" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="F17" s="43">
+      <c r="F17" s="40">
         <v>8</v>
       </c>
-      <c r="G17" s="43">
+      <c r="G17" s="40">
         <v>2</v>
       </c>
       <c r="H17" s="31">
@@ -2719,13 +2647,13 @@
       <c r="D18" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="43" t="s">
+      <c r="E18" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="F18" s="43">
+      <c r="F18" s="40">
         <v>8</v>
       </c>
-      <c r="G18" s="43">
+      <c r="G18" s="40">
         <v>2</v>
       </c>
       <c r="H18" s="31">
@@ -2753,13 +2681,13 @@
       <c r="D19" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="43" t="s">
+      <c r="E19" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="F19" s="43">
+      <c r="F19" s="40">
         <v>8</v>
       </c>
-      <c r="G19" s="43">
+      <c r="G19" s="40">
         <v>2</v>
       </c>
       <c r="H19" s="31">
@@ -2787,13 +2715,13 @@
       <c r="D20" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="43" t="s">
+      <c r="E20" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="F20" s="43">
+      <c r="F20" s="40">
         <v>5</v>
       </c>
-      <c r="G20" s="43">
+      <c r="G20" s="40">
         <v>1</v>
       </c>
       <c r="H20" s="12">
@@ -2819,13 +2747,13 @@
       <c r="D21" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="43" t="s">
+      <c r="E21" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="F21" s="43">
+      <c r="F21" s="40">
         <v>8</v>
       </c>
-      <c r="G21" s="43">
+      <c r="G21" s="40">
         <v>1</v>
       </c>
       <c r="H21" s="31">
@@ -2851,13 +2779,13 @@
       <c r="D22" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="43" t="s">
+      <c r="E22" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="F22" s="43">
+      <c r="F22" s="40">
         <v>8</v>
       </c>
-      <c r="G22" s="43">
+      <c r="G22" s="40">
         <v>2</v>
       </c>
       <c r="H22" s="31">
@@ -2874,7 +2802,7 @@
       <c r="A23" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="41" t="s">
         <v>61</v>
       </c>
       <c r="C23" s="30">
@@ -2883,13 +2811,13 @@
       <c r="D23" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="43" t="s">
+      <c r="E23" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="F23" s="43">
+      <c r="F23" s="40">
         <v>8</v>
       </c>
-      <c r="G23" s="43">
+      <c r="G23" s="40">
         <v>3</v>
       </c>
       <c r="H23" s="31">
@@ -2906,7 +2834,7 @@
       <c r="A24" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="41" t="s">
         <v>62</v>
       </c>
       <c r="C24" s="30">
@@ -2915,13 +2843,13 @@
       <c r="D24" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="43" t="s">
+      <c r="E24" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="F24" s="43">
+      <c r="F24" s="40">
         <v>13</v>
       </c>
-      <c r="G24" s="43">
+      <c r="G24" s="40">
         <v>3</v>
       </c>
       <c r="H24" s="31">
@@ -2938,7 +2866,7 @@
       <c r="A25" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="44" t="s">
+      <c r="B25" s="41" t="s">
         <v>63</v>
       </c>
       <c r="C25" s="30">
@@ -2947,13 +2875,13 @@
       <c r="D25" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="43" t="s">
+      <c r="E25" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="F25" s="43">
+      <c r="F25" s="40">
         <v>13</v>
       </c>
-      <c r="G25" s="43">
+      <c r="G25" s="40">
         <v>3</v>
       </c>
       <c r="H25" s="31">
@@ -2979,13 +2907,13 @@
       <c r="D26" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="43" t="s">
+      <c r="E26" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="F26" s="43">
+      <c r="F26" s="40">
         <v>8</v>
       </c>
-      <c r="G26" s="43">
+      <c r="G26" s="40">
         <v>3</v>
       </c>
       <c r="H26" s="31">
@@ -2998,7 +2926,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="34.799999999999997" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="19" t="s">
         <v>33</v>
       </c>
@@ -3028,7 +2956,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="33.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="22" t="s">
         <v>34</v>
       </c>
@@ -3058,7 +2986,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="34.799999999999997" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="22" t="s">
         <v>35</v>
       </c>
@@ -3088,7 +3016,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="34.799999999999997" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="22" t="s">
         <v>37</v>
       </c>
@@ -3118,7 +3046,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" ht="31.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="22" t="s">
         <v>38</v>
       </c>
@@ -3148,7 +3076,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="34.799999999999997" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="22" t="s">
         <v>39</v>
       </c>
@@ -3178,7 +3106,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="34.799999999999997" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="34.799999999999997" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="22" t="s">
         <v>40</v>
       </c>
@@ -3208,7 +3136,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="40.200000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="22" t="s">
         <v>41</v>
       </c>
@@ -3238,17 +3166,23 @@
         <v>82</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="B36" s="2"/>
     </row>
-    <row r="37" spans="1:10" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="32.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:G37" xr:uid="{68E230A6-6E41-41E9-834E-469679204ECD}"/>
+  <autoFilter ref="A2:G37" xr:uid="{68E230A6-6E41-41E9-834E-469679204ECD}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="2"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
   </mergeCells>
@@ -3263,6 +3197,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD11765F9AC0004AAF0A4CAAFDFAF16A" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b51fd1e8b3b325edc2e3e5af1016e876">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9fdc8751-6fef-42ec-b05c-835dd8c535b4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f375ab854fe714e6d25c0e520c080200" ns3:_="">
     <xsd:import namespace="9fdc8751-6fef-42ec-b05c-835dd8c535b4"/>
@@ -3438,15 +3381,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3454,6 +3388,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{085FFE83-7874-4863-A9C7-9C338481B563}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA33053E-EA8F-437C-9F67-47A4F0BC10D0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3467,14 +3409,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{085FFE83-7874-4863-A9C7-9C338481B563}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>